<commit_message>
Amelioration du model logique 5e2c24a1d6fe022a468036e3490e6708b6e34cbf
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-PatientId.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-PatientId.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-01T16:30:13+00:00</t>
+    <t>2025-05-02T13:48:14+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -248,7 +248,7 @@
     <t>Base</t>
   </si>
   <si>
-    <t>PatientId.CX1</t>
+    <t>PatientId.1</t>
   </si>
   <si>
     <t>1</t>
@@ -261,7 +261,7 @@
     <t>Identifiant du patient, en l’occurrence, le matricule INS du patient tel que défini dans le cadre juridique</t>
   </si>
   <si>
-    <t>PatientId.CX4</t>
+    <t>PatientId.4</t>
   </si>
   <si>
     <t xml:space="preserve">string
@@ -271,7 +271,7 @@
     <t>Identifiant de l’autorité d’affectation de l’INS utilisé.</t>
   </si>
   <si>
-    <t>PatientId.CX5</t>
+    <t>PatientId.5</t>
   </si>
   <si>
     <t xml:space="preserve"> 'NH' pour un maticule INS tel que défini dans le cadre juridique</t>
@@ -588,8 +588,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.57421875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.57421875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="9.3984375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.3984375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="7.6796875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
@@ -619,7 +619,7 @@
     <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="11.57421875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="9.91015625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>

</xml_diff>